<commit_message>
Fix budget file alignment with Pritzker template
- Corrected row 3 to show date only (removed leftover template text)
- Ensured Year 1/2/3 labels align with template format
- Year 1: 11/01/2025 to 10/31/2026
- Years 2 & 3: Empty (1-year grant)

Budget structure now matches template exactly.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/financials/PolicyEngine_Pritzker_Budget.xlsx
+++ b/financials/PolicyEngine_Pritzker_Budget.xlsx
@@ -1522,10 +1522,14 @@
       <c r="C1" s="144" t="n"/>
       <c r="E1" s="2" t="inlineStr">
         <is>
+          <t>YEAR 1 DATES</t>
+        </is>
+      </c>
+      <c r="F1" s="118" t="inlineStr">
+        <is>
           <t>11/01/2025 to 10/31/2026</t>
         </is>
       </c>
-      <c r="F1" s="118" t="inlineStr"/>
       <c r="G1" s="144" t="n"/>
     </row>
     <row r="2">
@@ -1536,7 +1540,11 @@
       </c>
       <c r="B2" s="146" t="n"/>
       <c r="C2" s="147" t="n"/>
-      <c r="E2" s="4" t="inlineStr"/>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>YEAR 2 DATES</t>
+        </is>
+      </c>
       <c r="F2" s="120" t="inlineStr"/>
       <c r="G2" s="147" t="n"/>
     </row>
@@ -1553,11 +1561,7 @@
           <t>YEAR 3 DATES</t>
         </is>
       </c>
-      <c r="F3" s="122" t="inlineStr">
-        <is>
-          <t>DD/MM/YY to DD/MM/YY</t>
-        </is>
-      </c>
+      <c r="F3" s="122" t="inlineStr"/>
       <c r="G3" s="150" t="n"/>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Add total organization revenue to budget
- Set B37 (Total Org. Revenue) to $1,000,000
- Reflects PSL Foundation's FY2026 budgeted revenue

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/financials/PolicyEngine_Pritzker_Budget.xlsx
+++ b/financials/PolicyEngine_Pritzker_Budget.xlsx
@@ -2161,10 +2161,8 @@
           <t>Total Org. Revenue***</t>
         </is>
       </c>
-      <c r="B37" s="163" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
+      <c r="B37" s="163" t="n">
+        <v>1000000</v>
       </c>
       <c r="D37" s="32" t="inlineStr">
         <is>

</xml_diff>